<commit_message>
Predicciones, similaciones y cumplimientos 2.0
</commit_message>
<xml_diff>
--- a/Proyecto1_Limpieza/emisiones_chilexpress.xlsx
+++ b/Proyecto1_Limpieza/emisiones_chilexpress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/506a708389be33d1/Escritorio/portafolio_chilexpress/Proyecto1_Limpieza/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="11_AD4D2F04E46CFB4ACB3E209DDDD3EBD6693EDF13" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A151B32-B5C6-4578-8417-6B093FF5FC56}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="11_AD4D2F04E46CFB4ACB3E209DDDD3EBD6693EDF13" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E947FE1-2E57-4CC3-8467-17BFA5A87BCC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -336,6 +336,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>